<commit_message>
added PD for all drugs, EMB bug still present
</commit_message>
<xml_diff>
--- a/Outputs/RIF/Tables/popPK_metric_analysis.xlsx
+++ b/Outputs/RIF/Tables/popPK_metric_analysis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1786" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1843" uniqueCount="136">
   <si>
     <t>Day 4, n = 100</t>
   </si>
@@ -753,7 +753,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0">
-        <v>113.08</v>
+        <v>113.09999999999999</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -767,7 +767,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>9.8300000000000001</v>
+        <v>10.5</v>
       </c>
       <c r="D3" s="0">
         <v>0</v>
@@ -781,7 +781,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>115.28</v>
+        <v>115.3</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
@@ -795,7 +795,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>13.529999999999999</v>
+        <v>14.390000000000001</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="0">
-        <v>3.69</v>
+        <v>3.8900000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restructured code to have a central script to run all drugs
</commit_message>
<xml_diff>
--- a/Outputs/RIF/Tables/popPK_metric_analysis.xlsx
+++ b/Outputs/RIF/Tables/popPK_metric_analysis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1957" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2071" uniqueCount="137">
   <si>
     <t>Day 4, n = 100</t>
   </si>
@@ -488,7 +488,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>5</v>
@@ -508,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0">
-        <v>193.53999999999999</v>
+        <v>167.36000000000001</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -522,7 +522,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>16.829999999999998</v>
+        <v>16.11</v>
       </c>
       <c r="D3" s="0">
         <v>0</v>
@@ -536,7 +536,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>200.6</v>
+        <v>174.25999999999999</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
@@ -550,7 +550,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>31.850000000000001</v>
+        <v>30.59</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
@@ -577,7 +577,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="0">
-        <v>7.0499999999999998</v>
+        <v>6.9000000000000004</v>
       </c>
     </row>
     <row r="8">
@@ -589,7 +589,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="0">
-        <v>15.02</v>
+        <v>14.48</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +612,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>5</v>
@@ -632,7 +632,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0">
-        <v>226.96000000000001</v>
+        <v>195.85</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>21.780000000000001</v>
+        <v>20.260000000000002</v>
       </c>
       <c r="D3" s="0">
         <v>0</v>
@@ -660,7 +660,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>222.05000000000001</v>
+        <v>190.80000000000001</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
@@ -674,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>30.68</v>
+        <v>29.809999999999999</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="0">
-        <v>4.9100000000000001</v>
+        <v>5.0499999999999998</v>
       </c>
     </row>
     <row r="8">
@@ -713,7 +713,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="0">
-        <v>8.9000000000000004</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +860,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>5</v>
@@ -880,7 +880,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0">
-        <v>106.67</v>
+        <v>95.409999999999997</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -894,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>8.2799999999999994</v>
+        <v>7.4800000000000004</v>
       </c>
       <c r="D3" s="0">
         <v>0</v>
@@ -908,7 +908,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>111.59999999999999</v>
+        <v>99.299999999999997</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
@@ -922,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>8.3499999999999997</v>
+        <v>7.4100000000000001</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
@@ -949,7 +949,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="0">
-        <v>4.9299999999999997</v>
+        <v>3.8900000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -958,7 +958,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0">
         <v>0.070000000000000007</v>

</xml_diff>

<commit_message>
reformatted to only one script to run the whole model
</commit_message>
<xml_diff>
--- a/Outputs/RIF/Tables/popPK_metric_analysis.xlsx
+++ b/Outputs/RIF/Tables/popPK_metric_analysis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2071" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2261" uniqueCount="150">
   <si>
     <t>Day 4, n = 100</t>
   </si>
@@ -429,6 +429,45 @@
   </si>
   <si>
     <t>Day 8, n = 1</t>
+  </si>
+  <si>
+    <t>Day 1, n = 2</t>
+  </si>
+  <si>
+    <t>Lung, p = 1.5393e-09</t>
+  </si>
+  <si>
+    <t>Lung, p = 3.93e-10</t>
+  </si>
+  <si>
+    <t>Lung, p = 4.8959e-09</t>
+  </si>
+  <si>
+    <t>Oral, p = 1.03e-10</t>
+  </si>
+  <si>
+    <t>Lung, p = 3.8437e-09</t>
+  </si>
+  <si>
+    <t>Lung, p = 5e-10</t>
+  </si>
+  <si>
+    <t>Lung, p = 7.8473e-10</t>
+  </si>
+  <si>
+    <t>Oral, p = 6.5e-11</t>
+  </si>
+  <si>
+    <t>Lung, p = 4.4466e-27</t>
+  </si>
+  <si>
+    <t>Lung, p = 1.48e-45</t>
+  </si>
+  <si>
+    <t>Lung, p = 4.7357e-30</t>
+  </si>
+  <si>
+    <t>Oral, p = 1.12e-35</t>
   </si>
 </sst>
 </file>
@@ -482,13 +521,13 @@
   <cols>
     <col min="1" max="1" width="14" customWidth="true"/>
     <col min="2" max="2" width="13.54296875" customWidth="true"/>
-    <col min="3" max="3" width="12.26953125" customWidth="true"/>
+    <col min="3" max="3" width="17.90625" customWidth="true"/>
     <col min="4" max="4" width="9.26953125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>5</v>
@@ -508,10 +547,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="0">
-        <v>167.36000000000001</v>
+        <v>177.61000000000001</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>55.049999999999997</v>
       </c>
     </row>
     <row r="3">
@@ -522,10 +561,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>16.11</v>
+        <v>16.149999999999999</v>
       </c>
       <c r="D3" s="0">
-        <v>0</v>
+        <v>1.8500000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -536,10 +575,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>174.25999999999999</v>
+        <v>183.15000000000001</v>
       </c>
       <c r="D4" s="0">
-        <v>0</v>
+        <v>53.049999999999997</v>
       </c>
     </row>
     <row r="5">
@@ -550,10 +589,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>30.59</v>
+        <v>30.670000000000002</v>
       </c>
       <c r="D5" s="0">
-        <v>0</v>
+        <v>5.5700000000000003</v>
       </c>
     </row>
     <row r="6">
@@ -574,10 +613,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="D7" s="0">
-        <v>6.9000000000000004</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="8">
@@ -586,10 +625,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
       <c r="D8" s="0">
-        <v>14.48</v>
+        <v>14.52</v>
       </c>
     </row>
   </sheetData>
@@ -606,13 +645,13 @@
   <cols>
     <col min="1" max="1" width="14" customWidth="true"/>
     <col min="2" max="2" width="13.54296875" customWidth="true"/>
-    <col min="3" max="3" width="12.26953125" customWidth="true"/>
+    <col min="3" max="3" width="17.90625" customWidth="true"/>
     <col min="4" max="4" width="9.26953125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>5</v>
@@ -632,10 +671,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="0">
-        <v>195.85</v>
+        <v>207.94</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>63.920000000000002</v>
       </c>
     </row>
     <row r="3">
@@ -646,10 +685,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>20.260000000000002</v>
+        <v>20.77</v>
       </c>
       <c r="D3" s="0">
-        <v>0</v>
+        <v>2.8300000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -660,10 +699,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>190.80000000000001</v>
+        <v>201.19999999999999</v>
       </c>
       <c r="D4" s="0">
-        <v>0</v>
+        <v>61.68</v>
       </c>
     </row>
     <row r="5">
@@ -674,10 +713,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>29.809999999999999</v>
+        <v>29.710000000000001</v>
       </c>
       <c r="D5" s="0">
-        <v>0</v>
+        <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="6">
@@ -698,10 +737,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>148</v>
       </c>
       <c r="D7" s="0">
-        <v>5.0499999999999998</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="8">
@@ -710,10 +749,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="D8" s="0">
-        <v>9.5500000000000007</v>
+        <v>8.9399999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>